<commit_message>
ch12 - multiple check box completed
</commit_message>
<xml_diff>
--- a/Challenge timsheet.xlsx
+++ b/Challenge timsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FRANKLIN\com.javascript30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D560AFEC-85FC-4E6C-926E-4B1461263AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D06D93-70A0-4727-8F56-2288E0CB5595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -154,6 +154,21 @@
   </si>
   <si>
     <t>Country Capital</t>
+  </si>
+  <si>
+    <t>Canvas</t>
+  </si>
+  <si>
+    <t>14 dev tools</t>
+  </si>
+  <si>
+    <t>multiple check box</t>
+  </si>
+  <si>
+    <t>Cuztom html5 video player</t>
+  </si>
+  <si>
+    <t>Key Sequence detection</t>
   </si>
 </sst>
 </file>
@@ -581,7 +596,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,9 +743,11 @@
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="E8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -744,9 +761,11 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="E9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -760,9 +779,11 @@
       <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E10" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -776,9 +797,11 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="E11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -792,7 +815,9 @@
       <c r="C12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="E12" s="5" t="s">
         <v>39</v>
       </c>
@@ -808,7 +833,9 @@
       <c r="C13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="E13" s="5" t="s">
         <v>39</v>
       </c>

</xml_diff>